<commit_message>
added a application database
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muj\IdeaProjects\EARS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09FA1E-13CC-4E15-9ED6-6460EF37C03F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1FB03A-0A95-475F-A0F1-E1025E16717A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="0" windowWidth="29040" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="29040" windowHeight="15600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logins" sheetId="1" r:id="rId1"/>
+    <sheet name="Applicants" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>admin</t>
   </si>
@@ -38,6 +39,126 @@
   </si>
   <si>
     <t>newpassword</t>
+  </si>
+  <si>
+    <t>taf</t>
+  </si>
+  <si>
+    <t>pass123</t>
+  </si>
+  <si>
+    <t>mmohmand</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>mohmand</t>
+  </si>
+  <si>
+    <t>10 Sunny Street, Toronto</t>
+  </si>
+  <si>
+    <t>mmohmand@algomau.ca</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>computer science</t>
+  </si>
+  <si>
+    <t>Algoma University</t>
+  </si>
+  <si>
+    <t>ceo</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>He's awesome!</t>
+  </si>
+  <si>
+    <t>C:\Users\muj\Desktop\algoma\Y Daniel Liang - Introduction to Java Programming and Data Structures, Comprehensive Version-Pearson (2017).pdf</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>jobid</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>degree</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>education</t>
+  </si>
+  <si>
+    <t>exp</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>communication</t>
+  </si>
+  <si>
+    <t>yearsexp</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jane </t>
+  </si>
+  <si>
+    <t>smith</t>
+  </si>
+  <si>
+    <t>123 fairway ave, sault ste marie, ontario</t>
+  </si>
+  <si>
+    <t>janesmith@google.com</t>
+  </si>
+  <si>
+    <t>555555555</t>
+  </si>
+  <si>
+    <t>Waterloo</t>
+  </si>
+  <si>
+    <t>developer</t>
+  </si>
+  <si>
+    <t>Good candiate. Recommended for interview with team.</t>
   </si>
 </sst>
 </file>
@@ -390,13 +511,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -409,7 +535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -420,7 +546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -429,6 +555,267 @@
       </c>
       <c r="C3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0A1740-D110-4DE6-8D42-3FA7FEF3F571}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>